<commit_message>
[PLAN] yesterday's plan was not completed because of the toothache.        today's main plan is to complete the reading of the chip manual
</commit_message>
<xml_diff>
--- a/Personal/xueyu/plan/周计划-2018-03-05.xlsx
+++ b/Personal/xueyu/plan/周计划-2018-03-05.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>今日计划</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,24 +58,73 @@
   </si>
   <si>
     <t>实际完成时间段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018/3/5
+周一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习qos芯片手册</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>背单词40个</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:10 - 12:35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:40 - 11:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成qos芯片手册的学习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习数学一节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英语阅读一篇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很多事，牙齿很痛，肿完了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018/3/6
+周二</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">本周总体规划：
 1. 抵制诱惑，本周不打游戏
-2. 学习qos的芯片手册和代码，思考出具体的修改实现方案
+2. 学习qos的芯片手册和代码，思考出具体的修改实现方案 （不做bcm了，要直接做es480的芯片，所以本周不一定都搞qos 2018-3-6 ）
 3. 完成单词和阅读任务
 4. 坚持完成数学的学习
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2018/3/5
-周一</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学习qos芯片手册</t>
+    <t>上午</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习qos芯片手册，尽快</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -83,23 +132,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>12:10 - 12:35</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10:40 - 11:40</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成qos芯片手册的学习</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学习数学一节</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>英语阅读一篇</t>
+    <t>下午</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重新读一遍，争取理解得更清楚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看一点点数学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>务必学习完成芯片手册，有什么不懂的赶紧问</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -419,22 +468,103 @@
     <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -455,6 +585,9 @@
     <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -467,98 +600,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -834,7 +883,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -842,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -860,22 +909,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="A1" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickTop="1">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="43"/>
+      <c r="B2" s="71"/>
       <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
@@ -896,427 +945,408 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="21" t="s">
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="68">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="67"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="69"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="64"/>
+      <c r="B5" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="40"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="73"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="41"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="37"/>
-      <c r="B5" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="41"/>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="69"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="69"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="64"/>
       <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="55"/>
+      <c r="H7" s="69"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="64"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="33"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="74"/>
+      <c r="E8" s="33"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="33"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="69"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="37"/>
-      <c r="B9" s="30" t="s">
+      <c r="A9" s="64"/>
+      <c r="B9" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="32"/>
+      <c r="E9" s="29"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="31"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="73"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="54"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="5"/>
+      <c r="A10" s="74" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="70"/>
+      <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="59"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="71"/>
+      <c r="H11" s="51"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="59"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="5"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="71"/>
+      <c r="H12" s="51"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="59"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="5"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="71"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="59"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="5"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="71"/>
+      <c r="H14" s="32"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="59"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="72"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="45"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="59"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="70"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="46"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="59"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="58"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="46"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="59"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="28"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="47"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="55"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="28"/>
+      <c r="A19" s="48"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="43"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="48"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="65"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="44"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="50"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="66"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="44"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="50"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="66"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="44"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="49"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="67"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="44"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="68"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="63"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="40"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="69"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="64"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="41"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="69"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="64"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="41"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="69"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="64"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="42"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="69"/>
-      <c r="B28" s="51"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="64"/>
+      <c r="A28" s="56"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="54"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="48"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="60"/>
+      <c r="A29" s="59"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="55"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="50"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="61"/>
+      <c r="A30" s="59"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="55"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="50"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="61"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="55"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="49"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="62"/>
+      <c r="A32" s="59"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="55"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="44"/>
-      <c r="B33" s="44"/>
+      <c r="A33" s="59"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
-      <c r="H33" s="52"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="45"/>
-      <c r="B34" s="45"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="47"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="45"/>
-      <c r="B35" s="51"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="47"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="45"/>
-      <c r="B36" s="46"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="47"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="45"/>
-      <c r="B37" s="47"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="47"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="45"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="47"/>
-    </row>
-    <row r="39" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A39" s="27"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="26"/>
+      <c r="H33" s="55"/>
+    </row>
+    <row r="34" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A34" s="27"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="A10:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="H29:H32"/>
-    <mergeCell ref="H24:H28"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="H10:H15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="H33:H38"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B33:B35"/>
+  <mergeCells count="25">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="A3:A9"/>
-    <mergeCell ref="H3:H5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:B4"/>
+    <mergeCell ref="G5:G9"/>
+    <mergeCell ref="H3:H9"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="H28:H33"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H19:H23"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="H10:H12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[week1 day3] [work] the main task of today is to complete the code reading of qos, and complete the code preparation of the adaptor chip [study] english and math learning
</commit_message>
<xml_diff>
--- a/Personal/xueyu/plan/周计划-2018-03-05.xlsx
+++ b/Personal/xueyu/plan/周计划-2018-03-05.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>今日计划</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -151,12 +151,61 @@
     <t>务必学习完成芯片手册，有什么不懂的赶紧问</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牙齿还痛，睡得很早</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上午</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习熟悉QOS代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下午</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>背单词40个</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习完成QOS代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如有剩余时间写完聚合口芯片配置的代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看一点数学，加油。或者看数学视频也行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018/3/7
+周三</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,15 +270,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="等线"/>
       <family val="3"/>
@@ -269,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -349,26 +389,6 @@
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -409,7 +429,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -427,34 +447,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="20" fontId="7" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -477,100 +480,100 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -588,12 +591,6 @@
     <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -603,10 +600,22 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -891,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B24" sqref="B24:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -909,32 +918,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickTop="1">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="62"/>
+      <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -945,13 +954,13 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -962,14 +971,14 @@
         <v>19</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="68">
+      <c r="H3" s="64">
         <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="67"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="21" t="s">
+      <c r="A4" s="60"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="15" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -980,11 +989,11 @@
         <v>19</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="69"/>
+      <c r="H4" s="65"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="64"/>
-      <c r="B5" s="63" t="s">
+      <c r="A5" s="57"/>
+      <c r="B5" s="56" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -995,68 +1004,68 @@
       <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="69"/>
+      <c r="H5" s="65"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="64"/>
-      <c r="B6" s="64"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="33"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="55"/>
-      <c r="H6" s="69"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="65"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="64"/>
-      <c r="B7" s="64"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="33"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="55"/>
-      <c r="H7" s="69"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="65"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="64"/>
-      <c r="B8" s="65"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="33"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="69"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="65"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="64"/>
-      <c r="B9" s="28" t="s">
+      <c r="A9" s="57"/>
+      <c r="B9" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="29"/>
+      <c r="E9" s="22"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="73"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="74" t="s">
+      <c r="G9" s="63"/>
+      <c r="H9" s="66"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A10" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="46" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1064,25 +1073,33 @@
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="50"/>
+      <c r="F10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="34">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="35"/>
-      <c r="B11" s="36"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="51"/>
+      <c r="F11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="38"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="35"/>
-      <c r="B12" s="30" t="s">
+      <c r="A12" s="33"/>
+      <c r="B12" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1090,13 +1107,15 @@
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="51"/>
+      <c r="F12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="38"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="35"/>
-      <c r="B13" s="52" t="s">
+      <c r="A13" s="33"/>
+      <c r="B13" s="48" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1104,224 +1123,206 @@
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="32"/>
+      <c r="F13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="38"/>
+      <c r="H13" s="35"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="31"/>
-      <c r="B14" s="53"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="32"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="45"/>
+      <c r="F14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="39"/>
+      <c r="H14" s="36"/>
+    </row>
+    <row r="15" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A15" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="30"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="38"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="46"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="38"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="46"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="31"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="39"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="47"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="31"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="48"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="43"/>
+      <c r="A19" s="68"/>
+      <c r="B19" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="31"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="49"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="44"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="27"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="49"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="44"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="28"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="49"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="44"/>
+      <c r="A22" s="53"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="28"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="49"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="44"/>
+      <c r="A23" s="52"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="29"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="37"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="40"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="44"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="38"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="14"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="41"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="45"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="38"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="14"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="13"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="41"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="45"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="39"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="14"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="42"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="45"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="56"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="54"/>
+      <c r="A28" s="42"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="45"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="59"/>
-      <c r="B29" s="59"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="55"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="59"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="55"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="59"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="55"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="59"/>
-      <c r="B32" s="55"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="55"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="59"/>
-      <c r="B33" s="55"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="55"/>
-    </row>
-    <row r="34" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A34" s="27"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="26"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="45"/>
+    </row>
+    <row r="30" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A30" s="20"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="22">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="A3:A9"/>
@@ -1329,24 +1330,21 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="G5:G9"/>
     <mergeCell ref="H3:H9"/>
-    <mergeCell ref="A28:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="H28:H33"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="H24:H29"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H19:H23"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="H10:H14"/>
+    <mergeCell ref="G10:G14"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B16:B18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[week6 day3] For the fist time since the chinese new year, I have learned a little bit of math and encourage myself to start again.
</commit_message>
<xml_diff>
--- a/Personal/xueyu/plan/周计划-2018-03-05.xlsx
+++ b/Personal/xueyu/plan/周计划-2018-03-05.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>今日计划</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -200,12 +200,24 @@
 周三</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看了空间向量的第一节的前四小节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,6 +501,84 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="7" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -503,6 +593,33 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -510,112 +627,7 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -892,21 +904,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:B26"/>
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
@@ -917,23 +929,23 @@
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:8" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickTop="1">
-      <c r="A2" s="61" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="62"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
@@ -953,11 +965,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="59" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -971,13 +983,13 @@
         <v>19</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="64">
+      <c r="H3" s="39">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="60"/>
-      <c r="B4" s="58"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="33"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="15" t="s">
         <v>12</v>
       </c>
@@ -989,11 +1001,11 @@
         <v>19</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="65"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="57"/>
-      <c r="B5" s="56" t="s">
+      <c r="H4" s="40"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="30"/>
+      <c r="B5" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1004,14 +1016,14 @@
       <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="50" t="s">
+      <c r="G5" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="65"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="57"/>
-      <c r="B6" s="57"/>
+      <c r="H5" s="40"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1020,12 +1032,12 @@
       <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="45"/>
-      <c r="H6" s="65"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="57"/>
-      <c r="B7" s="57"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="40"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1034,23 +1046,23 @@
       <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="45"/>
-      <c r="H7" s="65"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="57"/>
-      <c r="B8" s="58"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="40"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="30"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="24"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="65"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="57"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="40"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="30"/>
       <c r="B9" s="21" t="s">
         <v>7</v>
       </c>
@@ -1058,14 +1070,14 @@
       <c r="D9" s="4"/>
       <c r="E9" s="22"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="66"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A10" s="32" t="s">
+      <c r="G9" s="38"/>
+      <c r="H9" s="41"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="43" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1076,16 +1088,16 @@
       <c r="F10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="34">
+      <c r="H10" s="61">
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="33"/>
-      <c r="B11" s="47"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="68"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1094,11 +1106,11 @@
       <c r="F11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="33"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="62"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="68"/>
       <c r="B12" s="23" t="s">
         <v>26</v>
       </c>
@@ -1110,12 +1122,12 @@
       <c r="F12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="33"/>
-      <c r="B13" s="48" t="s">
+      <c r="G12" s="65"/>
+      <c r="H12" s="62"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="68"/>
+      <c r="B13" s="45" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1126,12 +1138,12 @@
       <c r="F13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="38"/>
-      <c r="H13" s="35"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="40"/>
-      <c r="B14" s="49"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="62"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="69"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
@@ -1140,11 +1152,11 @@
       <c r="F14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="39"/>
-      <c r="H14" s="36"/>
-    </row>
-    <row r="15" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A15" s="69" t="s">
+      <c r="G14" s="66"/>
+      <c r="H14" s="63"/>
+    </row>
+    <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="58" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="26" t="s">
@@ -1155,13 +1167,17 @@
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="9"/>
+      <c r="F15" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="30"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="67"/>
-      <c r="B16" s="41" t="s">
+      <c r="H15" s="56">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="59"/>
+      <c r="B16" s="47" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -1169,36 +1185,42 @@
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="F16" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="67"/>
-      <c r="B17" s="42"/>
+      <c r="H16" s="57"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="59"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="67"/>
-      <c r="B18" s="43"/>
+      <c r="H17" s="57"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="59"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="F18" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="G18" s="9"/>
-      <c r="H18" s="31"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="68"/>
+      <c r="H18" s="57"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="60"/>
       <c r="B19" s="25" t="s">
         <v>40</v>
       </c>
@@ -1207,111 +1229,115 @@
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="31"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="51"/>
+      <c r="F19" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="57"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="49"/>
       <c r="B20" s="17"/>
       <c r="C20" s="16"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
-      <c r="H20" s="27"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="53"/>
+      <c r="H20" s="53"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="51"/>
       <c r="B21" s="17"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
-      <c r="H21" s="28"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="53"/>
-      <c r="B22" s="51"/>
+      <c r="H21" s="54"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="51"/>
+      <c r="B22" s="49"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
-      <c r="H22" s="28"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="52"/>
-      <c r="B23" s="52"/>
+      <c r="H22" s="54"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="50"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
-      <c r="H23" s="29"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="41"/>
-      <c r="B24" s="41"/>
+      <c r="H23" s="55"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="47"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="44"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="42"/>
-      <c r="B25" s="42"/>
+      <c r="H24" s="42"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="48"/>
+      <c r="B25" s="48"/>
       <c r="C25" s="13"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
-      <c r="H25" s="45"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="42"/>
-      <c r="B26" s="43"/>
+      <c r="H25" s="37"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="48"/>
+      <c r="B26" s="52"/>
       <c r="C26" s="13"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="45"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="42"/>
-      <c r="B27" s="50"/>
+      <c r="H26" s="37"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="48"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="13"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
-      <c r="H27" s="45"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="42"/>
-      <c r="B28" s="45"/>
+      <c r="H27" s="37"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="48"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
-      <c r="H28" s="45"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="42"/>
-      <c r="B29" s="45"/>
+      <c r="H28" s="37"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="48"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
-      <c r="H29" s="45"/>
-    </row>
-    <row r="30" spans="1:8" ht="14.25" customHeight="1">
+      <c r="H29" s="37"/>
+    </row>
+    <row r="30" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20"/>
       <c r="B30" s="18"/>
       <c r="C30" s="11"/>
@@ -1323,13 +1349,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="G5:G9"/>
-    <mergeCell ref="H3:H9"/>
     <mergeCell ref="H24:H29"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B13:B14"/>
@@ -1345,6 +1364,13 @@
     <mergeCell ref="G10:G14"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="G5:G9"/>
+    <mergeCell ref="H3:H9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[week6 day4] today's task was all complete
</commit_message>
<xml_diff>
--- a/Personal/xueyu/plan/周计划-2018-03-05.xlsx
+++ b/Personal/xueyu/plan/周计划-2018-03-05.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F6E839-9678-48A9-8B15-B66AB86AD0DC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
   <si>
     <t>今日计划</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -273,8 +274,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -555,12 +556,60 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -579,14 +628,11 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -643,51 +689,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -964,21 +965,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
@@ -989,23 +990,23 @@
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:8" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickTop="1">
-      <c r="A2" s="63" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1025,11 +1026,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="61" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="30" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -1043,13 +1044,13 @@
         <v>19</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="66">
+      <c r="H3" s="40">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="62"/>
-      <c r="B4" s="60"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="34"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="15" t="s">
         <v>12</v>
       </c>
@@ -1061,11 +1062,11 @@
         <v>19</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="67"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="59"/>
-      <c r="B5" s="58" t="s">
+      <c r="H4" s="41"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="31"/>
+      <c r="B5" s="30" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1076,14 +1077,14 @@
       <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="67"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="59"/>
-      <c r="B6" s="59"/>
+      <c r="H5" s="41"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1092,12 +1093,12 @@
       <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="67"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="59"/>
-      <c r="B7" s="59"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="41"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1106,23 +1107,23 @@
       <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="67"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="59"/>
-      <c r="B8" s="60"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="41"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="31"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="23"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="67"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="59"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="41"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="31"/>
       <c r="B9" s="20" t="s">
         <v>7</v>
       </c>
@@ -1130,14 +1131,14 @@
       <c r="D9" s="4"/>
       <c r="E9" s="21"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="68"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A10" s="53" t="s">
+      <c r="G9" s="39"/>
+      <c r="H9" s="42"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="44" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1148,16 +1149,16 @@
       <c r="F10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="50" t="s">
+      <c r="G10" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="47">
+      <c r="H10" s="62">
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="54"/>
-      <c r="B11" s="29"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="69"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1166,11 +1167,11 @@
       <c r="F11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="51"/>
-      <c r="H11" s="48"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="54"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="63"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="69"/>
       <c r="B12" s="22" t="s">
         <v>26</v>
       </c>
@@ -1182,12 +1183,12 @@
       <c r="F12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="51"/>
-      <c r="H12" s="48"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="54"/>
-      <c r="B13" s="30" t="s">
+      <c r="G12" s="66"/>
+      <c r="H12" s="63"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="69"/>
+      <c r="B13" s="46" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1198,12 +1199,12 @@
       <c r="F13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="51"/>
-      <c r="H13" s="48"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="55"/>
-      <c r="B14" s="31"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="63"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="70"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
@@ -1212,11 +1213,11 @@
       <c r="F14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="52"/>
-      <c r="H14" s="49"/>
-    </row>
-    <row r="15" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A15" s="44" t="s">
+      <c r="G14" s="67"/>
+      <c r="H14" s="64"/>
+    </row>
+    <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="59" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="25" t="s">
@@ -1231,13 +1232,13 @@
         <v>42</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="42">
+      <c r="H15" s="57">
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="45"/>
-      <c r="B16" s="32" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="60"/>
+      <c r="B16" s="48" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -1249,11 +1250,11 @@
         <v>42</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="43"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="45"/>
-      <c r="B17" s="33"/>
+      <c r="H16" s="58"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="60"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1263,11 +1264,11 @@
         <v>43</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="43"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="45"/>
-      <c r="B18" s="38"/>
+      <c r="H17" s="58"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="60"/>
+      <c r="B18" s="53"/>
       <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
@@ -1277,10 +1278,10 @@
         <v>42</v>
       </c>
       <c r="G18" s="9"/>
-      <c r="H18" s="43"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="46"/>
+      <c r="H18" s="58"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="61"/>
       <c r="B19" s="24" t="s">
         <v>40</v>
       </c>
@@ -1295,13 +1296,13 @@
       <c r="G19" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H19" s="43"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="69" t="s">
+      <c r="H19" s="58"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="26" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="16" t="s">
@@ -1309,25 +1310,31 @@
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="F20" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="G20" s="11"/>
-      <c r="H20" s="39"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="70"/>
-      <c r="B21" s="36"/>
+      <c r="H20" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="51"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="16" t="s">
         <v>48</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="F21" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="G21" s="11"/>
-      <c r="H21" s="40"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="37"/>
-      <c r="B22" s="35" t="s">
+      <c r="H21" s="55"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="52"/>
+      <c r="B22" s="26" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -1337,13 +1344,15 @@
         <v>56</v>
       </c>
       <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+      <c r="F22" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="G22" s="11"/>
-      <c r="H22" s="40"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="37"/>
-      <c r="B23" s="36"/>
+      <c r="H22" s="55"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="52"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="11" t="s">
         <v>55</v>
       </c>
@@ -1351,13 +1360,15 @@
         <v>57</v>
       </c>
       <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
+      <c r="F23" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="G23" s="11"/>
-      <c r="H23" s="40"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="37"/>
-      <c r="B24" s="35" t="s">
+      <c r="H23" s="55"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="52"/>
+      <c r="B24" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C24" s="11" t="s">
@@ -1367,13 +1378,15 @@
         <v>58</v>
       </c>
       <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
+      <c r="F24" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="G24" s="11"/>
-      <c r="H24" s="40"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
+      <c r="H24" s="55"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="11" t="s">
         <v>52</v>
       </c>
@@ -1381,71 +1394,73 @@
         <v>59</v>
       </c>
       <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
+      <c r="F25" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="G25" s="11"/>
-      <c r="H25" s="41"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="32"/>
-      <c r="B26" s="32"/>
+      <c r="H25" s="56"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="48"/>
+      <c r="B26" s="48"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="26"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
+      <c r="H26" s="43"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="49"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="13"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
-      <c r="H27" s="27"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="33"/>
-      <c r="B28" s="38"/>
+      <c r="H27" s="38"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="49"/>
+      <c r="B28" s="53"/>
       <c r="C28" s="13"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
-      <c r="H28" s="27"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="33"/>
-      <c r="B29" s="34"/>
+      <c r="H28" s="38"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="49"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="13"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
-      <c r="H29" s="27"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="33"/>
-      <c r="B30" s="27"/>
+      <c r="H29" s="38"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="49"/>
+      <c r="B30" s="38"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
-      <c r="H30" s="27"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="33"/>
-      <c r="B31" s="27"/>
+      <c r="H30" s="38"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="49"/>
+      <c r="B31" s="38"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
-      <c r="H31" s="27"/>
-    </row>
-    <row r="32" spans="1:8" ht="14.25" customHeight="1">
+      <c r="H31" s="38"/>
+    </row>
+    <row r="32" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19"/>
       <c r="B32" s="17"/>
       <c r="C32" s="11"/>
@@ -1457,14 +1472,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="G5:G9"/>
-    <mergeCell ref="H3:H9"/>
     <mergeCell ref="H26:H31"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B13:B14"/>
@@ -1481,6 +1488,14 @@
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="G5:G9"/>
+    <mergeCell ref="H3:H9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[week6 day5] the morning's work is done satisfactorily, the afternoon is a little tight, come on.
</commit_message>
<xml_diff>
--- a/Personal/xueyu/plan/周计划-2018-03-05.xlsx
+++ b/Personal/xueyu/plan/周计划-2018-03-05.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
   <si>
     <t>今日计划</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -296,6 +296,78 @@
   </si>
   <si>
     <t>背单词40个</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9:20 - 10:14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下午</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搞清楚double模式怎么弄的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:00 - 14:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>今日总体目标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更换完成代码接口，适配新的sf芯片，为明天解决编译问题做准备。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:00 - 14:17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>也就是多申请一个临近的group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>把hsl首先recv到的消息看完并写完</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:40 - 17:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>把qos剩余内容写完</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:00 - 17:40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:50 - 18:20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>把ACL的接口替换完</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习高数空间向量第二节和第三节</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -407,7 +479,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -490,19 +562,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -527,7 +586,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -550,7 +609,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -563,127 +621,40 @@
     <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -707,20 +678,90 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1004,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26:H31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1017,27 +1058,28 @@
     <col min="3" max="3" width="48.625" customWidth="1"/>
     <col min="4" max="5" width="13.875" customWidth="1"/>
     <col min="6" max="6" width="14.375" customWidth="1"/>
-    <col min="7" max="7" width="30.125" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="30.125" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:9" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" thickTop="1">
-      <c r="A2" s="65" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickTop="1">
+      <c r="A2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="66"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1054,17 +1096,20 @@
         <v>4</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="63" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1075,14 +1120,15 @@
         <v>19</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="68">
+      <c r="H3" s="40"/>
+      <c r="I3" s="37">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="64"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="15" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4" s="34"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1093,11 +1139,12 @@
         <v>19</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="69"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="61"/>
-      <c r="B5" s="60" t="s">
+      <c r="H4" s="41"/>
+      <c r="I4" s="38"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="31"/>
+      <c r="B5" s="30" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1108,68 +1155,73 @@
       <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="69"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="61"/>
-      <c r="B6" s="61"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="38"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="23"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="69"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="61"/>
-      <c r="B7" s="61"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="38"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="23"/>
+      <c r="E7" s="20"/>
       <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="69"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="61"/>
-      <c r="B8" s="62"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="38"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="31"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="23"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="69"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="61"/>
-      <c r="B9" s="20" t="s">
+      <c r="G8" s="24"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="38"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="31"/>
+      <c r="B9" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="21"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="70"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A10" s="55" t="s">
+      <c r="G9" s="26"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="39"/>
+    </row>
+    <row r="10" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A10" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="49" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1180,16 +1232,17 @@
       <c r="F10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="49">
+      <c r="H10" s="51"/>
+      <c r="I10" s="52">
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="56"/>
-      <c r="B11" s="29"/>
+    <row r="11" spans="1:9">
+      <c r="A11" s="48"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1198,12 +1251,13 @@
       <c r="F11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="53"/>
-      <c r="H11" s="50"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="56"/>
-      <c r="B12" s="22" t="s">
+      <c r="G11" s="50"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="52"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="48"/>
+      <c r="B12" s="53" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1214,12 +1268,13 @@
       <c r="F12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="53"/>
-      <c r="H12" s="50"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="56"/>
-      <c r="B13" s="30" t="s">
+      <c r="G12" s="50"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="52"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="48"/>
+      <c r="B13" s="54" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1230,12 +1285,13 @@
       <c r="F13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="53"/>
-      <c r="H13" s="50"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="57"/>
-      <c r="B14" s="31"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="52"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="48"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
@@ -1244,17 +1300,18 @@
       <c r="F14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="54"/>
+      <c r="G14" s="50"/>
       <c r="H14" s="51"/>
-    </row>
-    <row r="15" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A15" s="46" t="s">
+      <c r="I14" s="52"/>
+    </row>
+    <row r="15" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A15" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="10"/>
@@ -1263,13 +1320,14 @@
         <v>42</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="44">
+      <c r="H15" s="9"/>
+      <c r="I15" s="56">
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="47"/>
-      <c r="B16" s="32" t="s">
+    <row r="16" spans="1:9">
+      <c r="A16" s="57"/>
+      <c r="B16" s="58" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -1281,25 +1339,27 @@
         <v>42</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="45"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="47"/>
-      <c r="B17" s="33"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="59"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="57"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="9"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="9" t="s">
         <v>43</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="45"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="47"/>
-      <c r="B18" s="40"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="59"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="57"/>
+      <c r="B18" s="58"/>
       <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
@@ -1309,11 +1369,12 @@
         <v>42</v>
       </c>
       <c r="G18" s="9"/>
-      <c r="H18" s="45"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="48"/>
-      <c r="B19" s="24" t="s">
+      <c r="H18" s="9"/>
+      <c r="I18" s="59"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="57"/>
+      <c r="B19" s="21" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1327,16 +1388,17 @@
       <c r="G19" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H19" s="45"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="37" t="s">
+      <c r="H19" s="9"/>
+      <c r="I19" s="59"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="11"/>
@@ -1345,14 +1407,15 @@
         <v>19</v>
       </c>
       <c r="G20" s="11"/>
-      <c r="H20" s="41">
+      <c r="H20" s="11"/>
+      <c r="I20" s="62">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="38"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="16" t="s">
+    <row r="21" spans="1:9">
+      <c r="A21" s="60"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="15" t="s">
         <v>48</v>
       </c>
       <c r="D21" s="11"/>
@@ -1361,11 +1424,12 @@
         <v>19</v>
       </c>
       <c r="G21" s="11"/>
-      <c r="H21" s="42"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="39"/>
-      <c r="B22" s="35" t="s">
+      <c r="H21" s="11"/>
+      <c r="I21" s="62"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="61"/>
+      <c r="B22" s="61" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -1379,11 +1443,12 @@
         <v>19</v>
       </c>
       <c r="G22" s="11"/>
-      <c r="H22" s="42"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="39"/>
-      <c r="B23" s="36"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="62"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="61"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="11" t="s">
         <v>55</v>
       </c>
@@ -1395,11 +1460,12 @@
         <v>19</v>
       </c>
       <c r="G23" s="11"/>
-      <c r="H23" s="42"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="39"/>
-      <c r="B24" s="35" t="s">
+      <c r="H23" s="11"/>
+      <c r="I23" s="62"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="61"/>
+      <c r="B24" s="61" t="s">
         <v>51</v>
       </c>
       <c r="C24" s="11" t="s">
@@ -1413,11 +1479,12 @@
         <v>19</v>
       </c>
       <c r="G24" s="11"/>
-      <c r="H24" s="42"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="62"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="61"/>
+      <c r="B25" s="61"/>
       <c r="C25" s="11" t="s">
         <v>52</v>
       </c>
@@ -1429,114 +1496,392 @@
         <v>19</v>
       </c>
       <c r="G25" s="11"/>
-      <c r="H25" s="43"/>
-    </row>
-    <row r="26" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A26" s="71" t="s">
+      <c r="H25" s="11"/>
+      <c r="I25" s="62"/>
+    </row>
+    <row r="26" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A26" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="26"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="27"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="13" t="s">
+      <c r="E26" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="12"/>
+      <c r="H26" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" s="64"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="42"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="27"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="27"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="13" t="s">
+      <c r="E27" s="13"/>
+      <c r="F27" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="12"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="65"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="42"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="27"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="27"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="27"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="27"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="67"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="27"/>
-    </row>
-    <row r="32" spans="1:8" ht="14.25" customHeight="1">
-      <c r="A32" s="19"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="18"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="12"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="65"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="42"/>
+      <c r="B29" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="63"/>
+      <c r="I29" s="65"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="42"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="65"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="42"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="65"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="42"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="65"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="43"/>
+      <c r="B33" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="46"/>
+    </row>
+    <row r="34" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A34" s="47"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="45"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="45"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="45"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="45"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="45"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="45"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="45"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="45"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="45"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="45"/>
+      <c r="B42" s="45"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="45"/>
+      <c r="B43" s="45"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="45"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="45"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="45"/>
+      <c r="B47" s="45"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="45"/>
+      <c r="G47" s="45"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="45"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="45"/>
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="45"/>
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="45"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="45"/>
+      <c r="B51" s="45"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="45"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="45"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="45"/>
+      <c r="B52" s="45"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="45"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="45"/>
+      <c r="B53" s="45"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="45"/>
+      <c r="F53" s="45"/>
+      <c r="G53" s="45"/>
+      <c r="H53" s="45"/>
+      <c r="I53" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
+    <mergeCell ref="H26:H32"/>
+    <mergeCell ref="A26:A33"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="G5:G9"/>
-    <mergeCell ref="H3:H9"/>
-    <mergeCell ref="H26:H31"/>
+    <mergeCell ref="I3:I9"/>
+    <mergeCell ref="I26:I32"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B29:B32"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A20:A25"/>
     <mergeCell ref="B26:B28"/>
-    <mergeCell ref="H20:H25"/>
-    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="I20:I25"/>
+    <mergeCell ref="I15:I19"/>
     <mergeCell ref="A15:A19"/>
-    <mergeCell ref="H10:H14"/>
+    <mergeCell ref="I10:I14"/>
     <mergeCell ref="G10:G14"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="B16:B18"/>

</xml_diff>

<commit_message>
[QOS] [plan] QOS is more complex than I think, and can't complete transplant it
</commit_message>
<xml_diff>
--- a/Personal/xueyu/plan/周计划-2018-03-05.xlsx
+++ b/Personal/xueyu/plan/周计划-2018-03-05.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18990" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="87">
   <si>
     <t>今日计划</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -323,10 +323,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>更换完成代码接口，适配新的sf芯片，为明天解决编译问题做准备。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>14:00 - 14:17</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -368,6 +364,19 @@
   </si>
   <si>
     <t>学习高数空间向量第二节和第三节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>还是挺复杂的，想多了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更换完成代码接口，适配新的sf芯片，为明天解决编译问题做准备。
+（想多了。。。）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -639,16 +648,41 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -678,6 +712,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -687,81 +730,47 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1037,7 +1046,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1047,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1063,23 +1072,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="36"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1103,10 +1112,10 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="39" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="14" t="s">
@@ -1120,14 +1129,14 @@
         <v>19</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="37">
+      <c r="H3" s="24"/>
+      <c r="I3" s="49">
         <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="34"/>
-      <c r="B4" s="32"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
@@ -1139,12 +1148,12 @@
         <v>19</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="38"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="50"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="31"/>
-      <c r="B5" s="30" t="s">
+      <c r="A5" s="40"/>
+      <c r="B5" s="39" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1155,15 +1164,15 @@
       <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="46" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="22"/>
-      <c r="I5" s="38"/>
+      <c r="I5" s="50"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1172,13 +1181,13 @@
       <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="24"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="22"/>
-      <c r="I6" s="38"/>
+      <c r="I6" s="50"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1187,25 +1196,25 @@
       <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="24"/>
+      <c r="G7" s="47"/>
       <c r="H7" s="22"/>
-      <c r="I7" s="38"/>
+      <c r="I7" s="50"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="31"/>
-      <c r="B8" s="32"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="20"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="24"/>
+      <c r="G8" s="47"/>
       <c r="H8" s="22"/>
-      <c r="I8" s="38"/>
+      <c r="I8" s="50"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="31"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="18" t="s">
         <v>7</v>
       </c>
@@ -1213,15 +1222,15 @@
       <c r="D9" s="4"/>
       <c r="E9" s="19"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="26"/>
+      <c r="G9" s="48"/>
       <c r="H9" s="23"/>
-      <c r="I9" s="39"/>
+      <c r="I9" s="51"/>
     </row>
     <row r="10" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="54" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1232,17 +1241,17 @@
       <c r="F10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="50" t="s">
+      <c r="G10" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="51"/>
-      <c r="I10" s="52">
+      <c r="H10" s="30"/>
+      <c r="I10" s="63">
         <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="48"/>
-      <c r="B11" s="49"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1251,13 +1260,13 @@
       <c r="F11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="52"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="63"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="48"/>
-      <c r="B12" s="53" t="s">
+      <c r="A12" s="65"/>
+      <c r="B12" s="31" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1268,13 +1277,13 @@
       <c r="F12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="50"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="52"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="63"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="48"/>
-      <c r="B13" s="54" t="s">
+      <c r="A13" s="65"/>
+      <c r="B13" s="55" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1285,13 +1294,13 @@
       <c r="F13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="50"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="63"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="48"/>
-      <c r="B14" s="54"/>
+      <c r="A14" s="65"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
@@ -1300,12 +1309,12 @@
       <c r="F14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="50"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="52"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="63"/>
     </row>
     <row r="15" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="61" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="21" t="s">
@@ -1321,13 +1330,13 @@
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
-      <c r="I15" s="56">
+      <c r="I15" s="59">
         <v>0.8</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="57"/>
-      <c r="B16" s="58" t="s">
+      <c r="A16" s="62"/>
+      <c r="B16" s="57" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -1340,11 +1349,11 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="59"/>
+      <c r="I16" s="60"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="57"/>
-      <c r="B17" s="58"/>
+      <c r="A17" s="62"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1355,11 +1364,11 @@
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
-      <c r="I17" s="59"/>
+      <c r="I17" s="60"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="57"/>
-      <c r="B18" s="58"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
@@ -1370,10 +1379,10 @@
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="59"/>
+      <c r="I18" s="60"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="57"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="21" t="s">
         <v>40</v>
       </c>
@@ -1389,13 +1398,13 @@
         <v>44</v>
       </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="59"/>
+      <c r="I19" s="60"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="36" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="15" t="s">
@@ -1408,13 +1417,13 @@
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="62">
+      <c r="I20" s="58">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="60"/>
-      <c r="B21" s="61"/>
+      <c r="A21" s="56"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="15" t="s">
         <v>48</v>
       </c>
@@ -1425,11 +1434,11 @@
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="62"/>
+      <c r="I21" s="58"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="61"/>
-      <c r="B22" s="61" t="s">
+      <c r="A22" s="36"/>
+      <c r="B22" s="36" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -1444,11 +1453,11 @@
       </c>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
-      <c r="I22" s="62"/>
+      <c r="I22" s="58"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="61"/>
-      <c r="B23" s="61"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="11" t="s">
         <v>55</v>
       </c>
@@ -1461,11 +1470,11 @@
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
-      <c r="I23" s="62"/>
+      <c r="I23" s="58"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="61"/>
-      <c r="B24" s="61" t="s">
+      <c r="A24" s="36"/>
+      <c r="B24" s="36" t="s">
         <v>51</v>
       </c>
       <c r="C24" s="11" t="s">
@@ -1480,11 +1489,11 @@
       </c>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
-      <c r="I24" s="62"/>
+      <c r="I24" s="58"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="61"/>
-      <c r="B25" s="61"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
       <c r="C25" s="11" t="s">
         <v>52</v>
       </c>
@@ -1497,13 +1506,13 @@
       </c>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
-      <c r="I25" s="62"/>
+      <c r="I25" s="58"/>
     </row>
     <row r="26" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="58" t="s">
+      <c r="B26" s="57" t="s">
         <v>61</v>
       </c>
       <c r="C26" s="12" t="s">
@@ -1519,14 +1528,14 @@
         <v>67</v>
       </c>
       <c r="G26" s="12"/>
-      <c r="H26" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="I26" s="64"/>
+      <c r="H26" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="I26" s="52"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="42"/>
-      <c r="B27" s="58"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="12" t="s">
         <v>65</v>
       </c>
@@ -1538,12 +1547,12 @@
         <v>67</v>
       </c>
       <c r="G27" s="12"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="65"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="53"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="42"/>
-      <c r="B28" s="58"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="57"/>
       <c r="C28" s="12" t="s">
         <v>66</v>
       </c>
@@ -1553,12 +1562,12 @@
         <v>67</v>
       </c>
       <c r="G28" s="12"/>
-      <c r="H28" s="63"/>
-      <c r="I28" s="65"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="53"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="42"/>
-      <c r="B29" s="65" t="s">
+      <c r="A29" s="34"/>
+      <c r="B29" s="53" t="s">
         <v>69</v>
       </c>
       <c r="C29" s="12" t="s">
@@ -1568,79 +1577,87 @@
         <v>71</v>
       </c>
       <c r="E29" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="G29" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="H29" s="32"/>
+      <c r="I29" s="53"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="34"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="H29" s="63"/>
-      <c r="I29" s="65"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="42"/>
-      <c r="B30" s="65"/>
-      <c r="C30" s="12" t="s">
+      <c r="D30" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="E30" s="12"/>
+      <c r="F30" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="H30" s="32"/>
+      <c r="I30" s="53"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="34"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="63"/>
-      <c r="I30" s="65"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="42"/>
-      <c r="B31" s="65"/>
-      <c r="C31" s="12" t="s">
+      <c r="D31" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="E31" s="12"/>
+      <c r="F31" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G31" s="47"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="53"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="34"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="63"/>
-      <c r="I31" s="65"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="42"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="12" t="s">
+      <c r="E32" s="12"/>
+      <c r="F32" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G32" s="48"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="53"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="35"/>
+      <c r="B33" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="65"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="43"/>
-      <c r="B33" s="46" t="s">
+      <c r="C33" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>84</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="46"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A34" s="47"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="16"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -1651,216 +1668,226 @@
       <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="45"/>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="45"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="45"/>
-      <c r="B36" s="45"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="45"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="45"/>
-      <c r="B38" s="45"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="45"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="45"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="45"/>
-      <c r="B39" s="45"/>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="45"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="45"/>
-      <c r="B40" s="45"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="45"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="45"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="45"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="45"/>
-      <c r="B42" s="45"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="45"/>
-      <c r="B43" s="45"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="45"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="45"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="45"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="45"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="45"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="27"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="45"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="45"/>
-      <c r="I48" s="45"/>
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="45"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="45"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="27"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="45"/>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="45"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="45"/>
-      <c r="B51" s="45"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-      <c r="G51" s="45"/>
-      <c r="H51" s="45"/>
-      <c r="I51" s="45"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="27"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="45"/>
-      <c r="B52" s="45"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
-      <c r="F52" s="45"/>
-      <c r="G52" s="45"/>
-      <c r="H52" s="45"/>
-      <c r="I52" s="45"/>
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="27"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="45"/>
-      <c r="B53" s="45"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="45"/>
-      <c r="F53" s="45"/>
-      <c r="G53" s="45"/>
-      <c r="H53" s="45"/>
-      <c r="I53" s="45"/>
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="27"/>
+      <c r="I53" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
+    <mergeCell ref="G30:G32"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="I20:I25"/>
+    <mergeCell ref="I15:I19"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="I10:I14"/>
+    <mergeCell ref="G10:G14"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="H26:H32"/>
     <mergeCell ref="A26:A33"/>
     <mergeCell ref="B22:B23"/>
@@ -1877,15 +1904,6 @@
     <mergeCell ref="B29:B32"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A20:A25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="I20:I25"/>
-    <mergeCell ref="I15:I19"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="I10:I14"/>
-    <mergeCell ref="G10:G14"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[week7 day1] the main goal this week is to remove the game. The goal today is to write code so that is can start compiling.
</commit_message>
<xml_diff>
--- a/Personal/xueyu/plan/周计划-2018-03-05.xlsx
+++ b/Personal/xueyu/plan/周计划-2018-03-05.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="98">
   <si>
     <t>今日计划</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -419,6 +419,10 @@
   <si>
     <t>更换完成代码接口，适配新的sf芯片，为下周解决编译问题做准备
 （ACL接口太多了，下周搞）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -700,13 +704,118 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -717,111 +826,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1097,7 +1101,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1107,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1123,23 +1127,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="76.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="42"/>
+      <c r="B2" s="62"/>
       <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1163,10 +1167,10 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="56" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="14" t="s">
@@ -1181,13 +1185,13 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="22"/>
-      <c r="I3" s="43">
+      <c r="I3" s="63">
         <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="40"/>
-      <c r="B4" s="38"/>
+      <c r="A4" s="60"/>
+      <c r="B4" s="58"/>
       <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
@@ -1200,11 +1204,11 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="23"/>
-      <c r="I4" s="44"/>
+      <c r="I4" s="64"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="37"/>
-      <c r="B5" s="36" t="s">
+      <c r="A5" s="57"/>
+      <c r="B5" s="56" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1215,15 +1219,15 @@
       <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="28" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="20"/>
-      <c r="I5" s="44"/>
+      <c r="I5" s="64"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1232,13 +1236,13 @@
       <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="66"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="20"/>
-      <c r="I6" s="44"/>
+      <c r="I6" s="64"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1247,25 +1251,25 @@
       <c r="F7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="66"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="20"/>
-      <c r="I7" s="44"/>
+      <c r="I7" s="64"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="18"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="66"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="20"/>
-      <c r="I8" s="44"/>
+      <c r="I8" s="64"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="37"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="16" t="s">
         <v>7</v>
       </c>
@@ -1273,15 +1277,15 @@
       <c r="D9" s="4"/>
       <c r="E9" s="17"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="67"/>
+      <c r="G9" s="30"/>
       <c r="H9" s="21"/>
-      <c r="I9" s="45"/>
+      <c r="I9" s="65"/>
     </row>
     <row r="10" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="51" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1292,17 +1296,17 @@
       <c r="F10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="68" t="s">
+      <c r="G10" s="49" t="s">
         <v>33</v>
       </c>
       <c r="H10" s="26"/>
-      <c r="I10" s="46">
+      <c r="I10" s="48">
         <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="47"/>
-      <c r="B11" s="49"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1311,12 +1315,12 @@
       <c r="F11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="68"/>
+      <c r="G11" s="49"/>
       <c r="H11" s="26"/>
-      <c r="I11" s="46"/>
+      <c r="I11" s="48"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="47"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="27" t="s">
         <v>26</v>
       </c>
@@ -1328,13 +1332,13 @@
       <c r="F12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="68"/>
+      <c r="G12" s="49"/>
       <c r="H12" s="26"/>
-      <c r="I12" s="46"/>
+      <c r="I12" s="48"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="47"/>
-      <c r="B13" s="50" t="s">
+      <c r="A13" s="50"/>
+      <c r="B13" s="52" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -1345,13 +1349,13 @@
       <c r="F13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="68"/>
+      <c r="G13" s="49"/>
       <c r="H13" s="26"/>
-      <c r="I13" s="46"/>
+      <c r="I13" s="48"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="47"/>
-      <c r="B14" s="50"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
@@ -1360,12 +1364,12 @@
       <c r="F14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="68"/>
+      <c r="G14" s="49"/>
       <c r="H14" s="26"/>
-      <c r="I14" s="46"/>
+      <c r="I14" s="48"/>
     </row>
     <row r="15" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="35" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="19" t="s">
@@ -1381,13 +1385,13 @@
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
-      <c r="I15" s="51">
+      <c r="I15" s="33">
         <v>0.8</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="54"/>
-      <c r="B16" s="48" t="s">
+      <c r="A16" s="36"/>
+      <c r="B16" s="31" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -1400,11 +1404,11 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="52"/>
+      <c r="I16" s="34"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="54"/>
-      <c r="B17" s="48"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1415,11 +1419,11 @@
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
-      <c r="I17" s="52"/>
+      <c r="I17" s="34"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="54"/>
-      <c r="B18" s="48"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
@@ -1430,10 +1434,10 @@
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="52"/>
+      <c r="I18" s="34"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="54"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="19" t="s">
         <v>40</v>
       </c>
@@ -1449,13 +1453,13 @@
         <v>44</v>
       </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="52"/>
+      <c r="I19" s="34"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="40" t="s">
         <v>47</v>
       </c>
       <c r="C20" s="15" t="s">
@@ -1468,13 +1472,13 @@
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="30">
+      <c r="I20" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="28"/>
-      <c r="B21" s="29"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="40"/>
       <c r="C21" s="15" t="s">
         <v>48</v>
       </c>
@@ -1485,11 +1489,11 @@
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="30"/>
+      <c r="I21" s="32"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29" t="s">
+      <c r="A22" s="40"/>
+      <c r="B22" s="40" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -1504,11 +1508,11 @@
       </c>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
-      <c r="I22" s="30"/>
+      <c r="I22" s="32"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
       <c r="C23" s="11" t="s">
         <v>55</v>
       </c>
@@ -1521,11 +1525,11 @@
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
-      <c r="I23" s="30"/>
+      <c r="I23" s="32"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="29"/>
-      <c r="B24" s="29" t="s">
+      <c r="A24" s="40"/>
+      <c r="B24" s="40" t="s">
         <v>51</v>
       </c>
       <c r="C24" s="11" t="s">
@@ -1540,11 +1544,11 @@
       </c>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
-      <c r="I24" s="30"/>
+      <c r="I24" s="32"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="11" t="s">
         <v>52</v>
       </c>
@@ -1557,13 +1561,13 @@
       </c>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
-      <c r="I25" s="30"/>
+      <c r="I25" s="32"/>
     </row>
     <row r="26" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="31" t="s">
         <v>61</v>
       </c>
       <c r="C26" s="12" t="s">
@@ -1579,16 +1583,16 @@
         <v>67</v>
       </c>
       <c r="G26" s="12"/>
-      <c r="H26" s="59" t="s">
+      <c r="H26" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="I26" s="62">
+      <c r="I26" s="45">
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="56"/>
-      <c r="B27" s="48"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="12" t="s">
         <v>65</v>
       </c>
@@ -1600,12 +1604,12 @@
         <v>67</v>
       </c>
       <c r="G27" s="12"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="63"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="46"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="56"/>
-      <c r="B28" s="48"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="12" t="s">
         <v>66</v>
       </c>
@@ -1615,12 +1619,12 @@
         <v>67</v>
       </c>
       <c r="G28" s="12"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="63"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="46"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="56"/>
-      <c r="B29" s="58" t="s">
+      <c r="A29" s="38"/>
+      <c r="B29" s="41" t="s">
         <v>69</v>
       </c>
       <c r="C29" s="12" t="s">
@@ -1638,12 +1642,12 @@
       <c r="G29" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H29" s="60"/>
-      <c r="I29" s="63"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="46"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="56"/>
-      <c r="B30" s="58"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="12" t="s">
         <v>76</v>
       </c>
@@ -1654,15 +1658,15 @@
       <c r="F30" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G30" s="65" t="s">
+      <c r="G30" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="H30" s="60"/>
-      <c r="I30" s="63"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="46"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="56"/>
-      <c r="B31" s="58"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="12" t="s">
         <v>86</v>
       </c>
@@ -1673,13 +1677,13 @@
       <c r="F31" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G31" s="66"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="63"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="46"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="56"/>
-      <c r="B32" s="58"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="12" t="s">
         <v>88</v>
       </c>
@@ -1690,12 +1694,12 @@
       <c r="F32" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="G32" s="67"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="63"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="46"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="57"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="25" t="s">
         <v>80</v>
       </c>
@@ -1708,14 +1712,14 @@
         <v>92</v>
       </c>
       <c r="G33" s="12"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="64"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="47"/>
     </row>
     <row r="34" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="40" t="s">
         <v>47</v>
       </c>
       <c r="C34" s="15" t="s">
@@ -1727,14 +1731,16 @@
         <v>93</v>
       </c>
       <c r="G34" s="11"/>
-      <c r="H34" s="31" t="s">
+      <c r="H34" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="I34" s="30"/>
+      <c r="I34" s="32">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="28"/>
-      <c r="B35" s="29"/>
+      <c r="A35" s="53"/>
+      <c r="B35" s="40"/>
       <c r="C35" s="15" t="s">
         <v>48</v>
       </c>
@@ -1744,12 +1750,12 @@
         <v>93</v>
       </c>
       <c r="G35" s="11"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="30"/>
+      <c r="H35" s="67"/>
+      <c r="I35" s="32"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29" t="s">
+      <c r="A36" s="40"/>
+      <c r="B36" s="40" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -1761,12 +1767,12 @@
         <v>93</v>
       </c>
       <c r="G36" s="11"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="30"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="32"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="11" t="s">
         <v>89</v>
       </c>
@@ -1778,12 +1784,12 @@
       <c r="G37" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="H37" s="32"/>
-      <c r="I37" s="30"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="32"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29" t="s">
+      <c r="A38" s="40"/>
+      <c r="B38" s="40" t="s">
         <v>27</v>
       </c>
       <c r="C38" s="11" t="s">
@@ -1791,23 +1797,27 @@
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
+      <c r="F38" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="G38" s="11"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="30"/>
+      <c r="H38" s="67"/>
+      <c r="I38" s="32"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="29"/>
-      <c r="B39" s="29"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="11" t="s">
         <v>91</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
+      <c r="F39" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="G39" s="11"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="30"/>
+      <c r="H39" s="68"/>
+      <c r="I39" s="32"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="24"/>
@@ -1965,6 +1975,27 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="I34:I39"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="H34:H39"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="G5:G9"/>
+    <mergeCell ref="I3:I9"/>
+    <mergeCell ref="I10:I14"/>
+    <mergeCell ref="G10:G14"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A20:A25"/>
     <mergeCell ref="G30:G32"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="I20:I25"/>
@@ -1976,27 +2007,6 @@
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="H26:H33"/>
     <mergeCell ref="I26:I33"/>
-    <mergeCell ref="I10:I14"/>
-    <mergeCell ref="G10:G14"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="G5:G9"/>
-    <mergeCell ref="I3:I9"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="I34:I39"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="H34:H39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>